<commit_message>
IFC file write minus tendon value done
</commit_message>
<xml_diff>
--- a/loadTables.xlsx
+++ b/loadTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +240,12 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -788,33 +794,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -823,6 +811,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1140,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM27"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1167,65 +1173,65 @@
   <sheetData>
     <row r="1" spans="1:39" ht="26.25" customHeight="1" thickBot="1">
       <c r="A1" s="7"/>
-      <c r="B1" s="105">
+      <c r="B1" s="106">
         <v>25</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="109">
+      <c r="C1" s="107"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="113">
         <v>35</v>
       </c>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="105">
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="106">
         <v>40</v>
       </c>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="105">
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="106">
         <v>50</v>
       </c>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="110">
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="114">
         <v>60</v>
       </c>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="110">
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="114">
         <v>70</v>
       </c>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="105">
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
+      <c r="AB1" s="115"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="106">
         <v>80</v>
       </c>
-      <c r="AE1" s="106"/>
-      <c r="AF1" s="106"/>
-      <c r="AG1" s="107"/>
+      <c r="AE1" s="107"/>
+      <c r="AF1" s="107"/>
+      <c r="AG1" s="111"/>
       <c r="AH1" s="36">
         <v>90</v>
       </c>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
-      <c r="AK1" s="108">
+      <c r="AK1" s="112">
         <v>100</v>
       </c>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="112"/>
     </row>
     <row r="2" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A2" s="114">
+      <c r="A2" s="108">
         <v>40</v>
       </c>
       <c r="B2" s="4"/>
@@ -1300,7 +1306,7 @@
       <c r="AM2" s="7"/>
     </row>
     <row r="3" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A3" s="115"/>
+      <c r="A3" s="109"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
@@ -1373,7 +1379,7 @@
       <c r="AM3" s="7"/>
     </row>
     <row r="4" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A4" s="114">
+      <c r="A4" s="108">
         <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1466,7 +1472,7 @@
       <c r="AM4" s="7"/>
     </row>
     <row r="5" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A5" s="115"/>
+      <c r="A5" s="109"/>
       <c r="B5" s="2">
         <v>6</v>
       </c>
@@ -1557,7 +1563,7 @@
       <c r="AM5" s="7"/>
     </row>
     <row r="6" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A6" s="114">
+      <c r="A6" s="108">
         <v>80</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1642,7 +1648,7 @@
       <c r="AM6" s="7"/>
     </row>
     <row r="7" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A7" s="115"/>
+      <c r="A7" s="109"/>
       <c r="B7" s="2">
         <v>6</v>
       </c>
@@ -1725,7 +1731,7 @@
       <c r="AM7" s="7"/>
     </row>
     <row r="8" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A8" s="114">
+      <c r="A8" s="108">
         <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1814,7 +1820,7 @@
       <c r="AM8" s="7"/>
     </row>
     <row r="9" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A9" s="115"/>
+      <c r="A9" s="109"/>
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -1901,7 +1907,7 @@
       <c r="AM9" s="7"/>
     </row>
     <row r="10" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A10" s="114">
+      <c r="A10" s="108">
         <v>250</v>
       </c>
       <c r="B10" s="4"/>
@@ -1964,7 +1970,7 @@
       <c r="AM10" s="7"/>
     </row>
     <row r="11" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A11" s="115"/>
+      <c r="A11" s="109"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="22">
@@ -2031,48 +2037,48 @@
       </c>
     </row>
     <row r="15" spans="1:39">
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="116"/>
-      <c r="L15" s="116"/>
-      <c r="M15" s="116"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="110"/>
+      <c r="L15" s="110"/>
+      <c r="M15" s="110"/>
     </row>
     <row r="16" spans="1:39">
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="116"/>
-      <c r="L16" s="116"/>
-      <c r="M16" s="116"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="110"/>
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="B17" s="116"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="116"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="110"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="110"/>
     </row>
     <row r="18" spans="1:13">
       <c r="B18" s="55" t="s">
@@ -2083,20 +2089,20 @@
       <c r="E18" s="55"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="H19" s="113" t="s">
+      <c r="H19" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="105"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="H20" s="113"/>
-      <c r="I20" s="113"/>
-      <c r="J20" s="113"/>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="105"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="56" t="s">
@@ -2196,6 +2202,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="X1:AC1"/>
     <mergeCell ref="H19:L20"/>
     <mergeCell ref="L1:Q1"/>
     <mergeCell ref="A2:A3"/>
@@ -2204,15 +2217,10 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B15:M17"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="X1:AC1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2225,7 +2233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5542,65 +5550,65 @@
   <sheetData>
     <row r="1" spans="1:39" ht="26.25" customHeight="1" thickBot="1">
       <c r="A1" s="57"/>
-      <c r="B1" s="105">
+      <c r="B1" s="106">
         <v>25</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="109">
+      <c r="C1" s="107"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="113">
         <v>35</v>
       </c>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="105">
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="106">
         <v>40</v>
       </c>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="105">
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="106">
         <v>50</v>
       </c>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="110">
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="114">
         <v>60</v>
       </c>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="110">
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="114">
         <v>70</v>
       </c>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="105">
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
+      <c r="AB1" s="115"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="106">
         <v>80</v>
       </c>
-      <c r="AE1" s="106"/>
-      <c r="AF1" s="106"/>
-      <c r="AG1" s="107"/>
+      <c r="AE1" s="107"/>
+      <c r="AF1" s="107"/>
+      <c r="AG1" s="111"/>
       <c r="AH1" s="36">
         <v>90</v>
       </c>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
-      <c r="AK1" s="108">
+      <c r="AK1" s="112">
         <v>100</v>
       </c>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="112"/>
     </row>
     <row r="2" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A2" s="114">
+      <c r="A2" s="108">
         <v>40</v>
       </c>
       <c r="B2" s="4"/>
@@ -5675,7 +5683,7 @@
       <c r="AM2" s="57"/>
     </row>
     <row r="3" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A3" s="115"/>
+      <c r="A3" s="109"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
@@ -5789,7 +5797,7 @@
       <c r="AM4" s="57"/>
     </row>
     <row r="5" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A5" s="114">
+      <c r="A5" s="108">
         <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -5882,7 +5890,7 @@
       <c r="AM5" s="57"/>
     </row>
     <row r="6" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A6" s="115"/>
+      <c r="A6" s="109"/>
       <c r="B6" s="2">
         <v>6</v>
       </c>
@@ -6012,7 +6020,7 @@
       <c r="AM7" s="57"/>
     </row>
     <row r="8" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A8" s="114">
+      <c r="A8" s="108">
         <v>80</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -6097,7 +6105,7 @@
       <c r="AM8" s="57"/>
     </row>
     <row r="9" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A9" s="115"/>
+      <c r="A9" s="109"/>
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -6221,7 +6229,7 @@
       <c r="AM10" s="57"/>
     </row>
     <row r="11" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A11" s="114">
+      <c r="A11" s="108">
         <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -6310,7 +6318,7 @@
       <c r="AM11" s="57"/>
     </row>
     <row r="12" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A12" s="115"/>
+      <c r="A12" s="109"/>
       <c r="B12" s="2">
         <v>6</v>
       </c>
@@ -6397,7 +6405,7 @@
       <c r="AM12" s="57"/>
     </row>
     <row r="13" spans="1:39" ht="20.25" customHeight="1">
-      <c r="A13" s="114">
+      <c r="A13" s="108">
         <v>250</v>
       </c>
       <c r="B13" s="4"/>
@@ -6460,7 +6468,7 @@
       <c r="AM13" s="57"/>
     </row>
     <row r="14" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A14" s="115"/>
+      <c r="A14" s="109"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="72">
@@ -6527,48 +6535,48 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="116"/>
-      <c r="L18" s="116"/>
-      <c r="M18" s="116"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="110"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="110"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="116"/>
-      <c r="K19" s="116"/>
-      <c r="L19" s="116"/>
-      <c r="M19" s="116"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="110"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="110"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="116"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
     </row>
     <row r="21" spans="1:13">
       <c r="B21" s="55" t="s">
@@ -6579,20 +6587,20 @@
       <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="H22" s="113" t="s">
+      <c r="H22" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="113"/>
-      <c r="J22" s="113"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="H23" s="113"/>
-      <c r="I23" s="113"/>
-      <c r="J23" s="113"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="113"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="56" t="s">

</xml_diff>